<commit_message>
Merged PR 1354: Updated TIBCO portion and added missing input vars
Updated TIBCO portion of script and template to improve formatting.  Added missing vars to QA sheet in input spreadsheet.

Related work items: #28703
</commit_message>
<xml_diff>
--- a/IRMA/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/IRMA/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="141">
   <si>
     <t>Key</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>CHG0033369</t>
+  </si>
+  <si>
+    <t>MammothPriceListener,R10PriceService</t>
   </si>
 </sst>
 </file>
@@ -820,9 +823,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1265,7 +1268,7 @@
         <v>91</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -1309,6 +1312,49 @@
       </c>
       <c r="C48" s="2" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1321,9 +1367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="A2:C53"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1377,7 @@
     <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.140625" customWidth="1"/>
     <col min="3" max="3" width="42.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1658,7 +1704,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -1751,7 +1797,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -1848,7 +1894,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>132</v>
       </c>

</xml_diff>